<commit_message>
22.05.2024 Part Exchange Change
</commit_message>
<xml_diff>
--- a/src/main/java/com/amt/testData/QuoteSave.xlsx
+++ b/src/main/java/com/amt/testData/QuoteSave.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="358">
   <si>
     <t xml:space="preserve">Quote Ref No</t>
   </si>
@@ -1101,6 +1101,12 @@
   </si>
   <si>
     <t>YWH65156</t>
+  </si>
+  <si>
+    <t>BHE09006</t>
+  </si>
+  <si>
+    <t>TTM54429</t>
   </si>
 </sst>
 </file>
@@ -2023,7 +2029,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2385,7 +2391,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>

</xml_diff>